<commit_message>
modified:   File_exists.py 	modified:   Maxpowerinputfile.xlsx 	modified:   Minpowerinputfile.xlsx
</commit_message>
<xml_diff>
--- a/Maxpowerinputfile.xlsx
+++ b/Maxpowerinputfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\RX_Spurious_Emission\New folder (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\LTE_RX_logging\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F566FEB-891D-4A04-8303-2F3A76E63576}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776D0133-6149-4105-8104-900F7D5C9253}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1335" windowWidth="25500" windowHeight="14265" activeTab="5" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
+    <workbookView xWindow="2925" yWindow="945" windowWidth="25500" windowHeight="14265" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>
   <sheets>
     <sheet name="Band2" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="19">
   <si>
     <t>Band</t>
   </si>
@@ -87,19 +87,16 @@
     <t>BAND 66</t>
   </si>
   <si>
-    <t>PASS/Fail</t>
+    <t>start_freq_rang1</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>start_freq_rang2</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>stop_freq_rang1</t>
   </si>
   <si>
-    <t>PASS/FAIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total No of Test Cases: </t>
+    <t>stop_freq_rang2</t>
   </si>
 </sst>
 </file>
@@ -111,7 +108,7 @@
     <numFmt numFmtId="165" formatCode="0;[Red]0"/>
     <numFmt numFmtId="166" formatCode="0_);\(0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,8 +150,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,24 +189,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +251,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -276,31 +262,11 @@
     <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="6" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="3" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="6" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="3" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="2" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -319,12 +285,11 @@
     <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -642,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89F21EF5-0615-4121-83E8-517FC8180B1A}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,10 +622,12 @@
     <col min="5" max="5" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
+    <col min="10" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -682,11 +649,20 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -708,8 +684,20 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>30000000</v>
+      </c>
+      <c r="I2">
+        <v>1000000000</v>
+      </c>
+      <c r="J2">
+        <v>1000000000</v>
+      </c>
+      <c r="K2">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>20</v>
       </c>
@@ -728,8 +716,20 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>30000000</v>
+      </c>
+      <c r="I3">
+        <v>1000000000</v>
+      </c>
+      <c r="J3">
+        <v>1000000000</v>
+      </c>
+      <c r="K3">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>20</v>
       </c>
@@ -747,6 +747,18 @@
       </c>
       <c r="G4" t="s">
         <v>9</v>
+      </c>
+      <c r="H4">
+        <v>30000000</v>
+      </c>
+      <c r="I4">
+        <v>1000000000</v>
+      </c>
+      <c r="J4">
+        <v>1000000000</v>
+      </c>
+      <c r="K4">
+        <v>12750000000</v>
       </c>
     </row>
   </sheetData>
@@ -761,10 +773,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855F8828-1D8C-4AAA-81FD-7AC3397EB1C9}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +787,8 @@
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -800,7 +813,16 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>18</v>
       </c>
     </row>
@@ -826,8 +848,17 @@
       <c r="G2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="54" t="s">
-        <v>16</v>
+      <c r="H2">
+        <v>30000000</v>
+      </c>
+      <c r="I2">
+        <v>1000000000</v>
+      </c>
+      <c r="J2">
+        <v>1000000000</v>
+      </c>
+      <c r="K2">
+        <v>12750000000</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -850,7 +881,18 @@
       <c r="G3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="54"/>
+      <c r="H3">
+        <v>30000000</v>
+      </c>
+      <c r="I3">
+        <v>1000000000</v>
+      </c>
+      <c r="J3">
+        <v>1000000000</v>
+      </c>
+      <c r="K3">
+        <v>12750000000</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -872,255 +914,18 @@
       <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="54"/>
-      <c r="J4" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="58">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="54"/>
-      <c r="J5" s="56" t="s">
-        <v>16</v>
-      </c>
-      <c r="K5" s="58">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="54"/>
-      <c r="J6" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="58">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="54"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="54"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="54"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="54"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="53"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="53"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="54"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="54"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="31"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="32"/>
-      <c r="H15" s="54"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="54"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="54"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="54"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="53"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="53"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="53"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="53"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="53"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="53"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="54"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="54"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="54"/>
+      <c r="H4">
+        <v>30000000</v>
+      </c>
+      <c r="I4">
+        <v>1000000000</v>
+      </c>
+      <c r="J4">
+        <v>1000000000</v>
+      </c>
+      <c r="K4">
+        <v>12750000000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1129,10 +934,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8596D56-7C71-4D72-A666-9CAEA981CBE7}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H1" sqref="H1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,36 +948,46 @@
     <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="8" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="56" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="56" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1194,8 +1009,20 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>30000000</v>
+      </c>
+      <c r="I2">
+        <v>1000000000</v>
+      </c>
+      <c r="J2">
+        <v>1000000000</v>
+      </c>
+      <c r="K2">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>10</v>
       </c>
@@ -1214,8 +1041,20 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>30000000</v>
+      </c>
+      <c r="I3">
+        <v>1000000000</v>
+      </c>
+      <c r="J3">
+        <v>1000000000</v>
+      </c>
+      <c r="K3">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>10</v>
       </c>
@@ -1233,6 +1072,18 @@
       </c>
       <c r="G4" t="s">
         <v>9</v>
+      </c>
+      <c r="H4">
+        <v>30000000</v>
+      </c>
+      <c r="I4">
+        <v>1000000000</v>
+      </c>
+      <c r="J4">
+        <v>1000000000</v>
+      </c>
+      <c r="K4">
+        <v>12750000000</v>
       </c>
     </row>
   </sheetData>
@@ -1246,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D108741B-A8D0-4BB3-B12C-6B68B68001DF}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,36 +1111,46 @@
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="9" max="9" width="21" customWidth="1"/>
+    <col min="10" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -1311,8 +1172,20 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>30000000</v>
+      </c>
+      <c r="I2">
+        <v>1000000000</v>
+      </c>
+      <c r="J2">
+        <v>1000000000</v>
+      </c>
+      <c r="K2">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>10</v>
       </c>
@@ -1331,8 +1204,20 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>30000000</v>
+      </c>
+      <c r="I3">
+        <v>1000000000</v>
+      </c>
+      <c r="J3">
+        <v>1000000000</v>
+      </c>
+      <c r="K3">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>10</v>
       </c>
@@ -1350,6 +1235,18 @@
       </c>
       <c r="G4" t="s">
         <v>9</v>
+      </c>
+      <c r="H4">
+        <v>30000000</v>
+      </c>
+      <c r="I4">
+        <v>1000000000</v>
+      </c>
+      <c r="J4">
+        <v>1000000000</v>
+      </c>
+      <c r="K4">
+        <v>12750000000</v>
       </c>
     </row>
   </sheetData>
@@ -1360,10 +1257,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7206B6-36E5-4637-B4E1-0FEA65E91330}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1373,10 +1270,11 @@
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1398,11 +1296,20 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>66</v>
       </c>
@@ -1424,8 +1331,20 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>30000000</v>
+      </c>
+      <c r="I2">
+        <v>1000000000</v>
+      </c>
+      <c r="J2">
+        <v>1000000000</v>
+      </c>
+      <c r="K2">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>20</v>
       </c>
@@ -1444,8 +1363,20 @@
       <c r="G3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>30000000</v>
+      </c>
+      <c r="I3">
+        <v>1000000000</v>
+      </c>
+      <c r="J3">
+        <v>1000000000</v>
+      </c>
+      <c r="K3">
+        <v>12750000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>20</v>
       </c>
@@ -1463,6 +1394,18 @@
       </c>
       <c r="G4" t="s">
         <v>9</v>
+      </c>
+      <c r="H4">
+        <v>30000000</v>
+      </c>
+      <c r="I4">
+        <v>1000000000</v>
+      </c>
+      <c r="J4">
+        <v>1000000000</v>
+      </c>
+      <c r="K4">
+        <v>12750000000</v>
       </c>
     </row>
   </sheetData>
@@ -1472,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDABD784-AD31-46F2-99DC-A4DD1B41AE1B}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,11 +1428,12 @@
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="29.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1511,11 +1455,20 @@
       <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="37" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>13</v>
       </c>
@@ -1536,6 +1489,18 @@
       </c>
       <c r="G2" t="s">
         <v>8</v>
+      </c>
+      <c r="H2">
+        <v>30000000</v>
+      </c>
+      <c r="I2">
+        <v>1000000000</v>
+      </c>
+      <c r="J2">
+        <v>1000000000</v>
+      </c>
+      <c r="K2">
+        <v>12750000000</v>
       </c>
     </row>
   </sheetData>
@@ -1582,900 +1547,900 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
+      <c r="A2" s="14">
         <v>2</v>
       </c>
-      <c r="B2" s="35">
+      <c r="B2" s="15">
         <v>20</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="16">
         <v>1940</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="17">
         <v>100</v>
       </c>
-      <c r="E2" s="37">
-        <v>0</v>
-      </c>
-      <c r="F2" s="36">
-        <v>23</v>
-      </c>
-      <c r="G2" s="35" t="s">
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
+      <c r="F2" s="16">
+        <v>23</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="35">
+      <c r="A3" s="14"/>
+      <c r="B3" s="15">
         <v>20</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="16">
         <v>1940</v>
       </c>
-      <c r="D3" s="37">
-        <v>1</v>
-      </c>
-      <c r="E3" s="37">
-        <v>0</v>
-      </c>
-      <c r="F3" s="36">
-        <v>23</v>
-      </c>
-      <c r="G3" s="35" t="s">
+      <c r="D3" s="17">
+        <v>1</v>
+      </c>
+      <c r="E3" s="17">
+        <v>0</v>
+      </c>
+      <c r="F3" s="16">
+        <v>23</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="35">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15">
         <v>20</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="16">
         <v>1940</v>
       </c>
-      <c r="D4" s="37">
-        <v>1</v>
-      </c>
-      <c r="E4" s="37">
+      <c r="D4" s="17">
+        <v>1</v>
+      </c>
+      <c r="E4" s="17">
         <v>99</v>
       </c>
-      <c r="F4" s="36">
-        <v>23</v>
-      </c>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="16">
+        <v>23</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
-      <c r="B5" s="38">
+      <c r="A5" s="14"/>
+      <c r="B5" s="18">
         <v>1.4</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="19">
         <v>1960</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="20">
         <v>6</v>
       </c>
-      <c r="E5" s="40">
-        <v>0</v>
-      </c>
-      <c r="F5" s="39">
-        <v>23</v>
-      </c>
-      <c r="G5" s="38" t="s">
+      <c r="E5" s="20">
+        <v>0</v>
+      </c>
+      <c r="F5" s="19">
+        <v>23</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
-      <c r="B6" s="41">
+      <c r="A6" s="14"/>
+      <c r="B6" s="21">
         <v>1.4</v>
       </c>
-      <c r="C6" s="42">
+      <c r="C6" s="22">
         <v>1960</v>
       </c>
-      <c r="D6" s="43">
-        <v>1</v>
-      </c>
-      <c r="E6" s="43">
-        <v>0</v>
-      </c>
-      <c r="F6" s="42">
-        <v>23</v>
-      </c>
-      <c r="G6" s="41" t="s">
+      <c r="D6" s="23">
+        <v>1</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0</v>
+      </c>
+      <c r="F6" s="22">
+        <v>23</v>
+      </c>
+      <c r="G6" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
-      <c r="B7" s="44">
+      <c r="A7" s="14"/>
+      <c r="B7" s="24">
         <v>1.4</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="25">
         <v>1960</v>
       </c>
-      <c r="D7" s="46">
-        <v>1</v>
-      </c>
-      <c r="E7" s="46">
+      <c r="D7" s="26">
+        <v>1</v>
+      </c>
+      <c r="E7" s="26">
         <v>5</v>
       </c>
-      <c r="F7" s="45">
-        <v>23</v>
-      </c>
-      <c r="G7" s="44" t="s">
+      <c r="F7" s="25">
+        <v>23</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
-      <c r="B8" s="44">
+      <c r="A8" s="14"/>
+      <c r="B8" s="24">
         <v>5</v>
       </c>
-      <c r="C8" s="45">
+      <c r="C8" s="25">
         <v>1960</v>
       </c>
-      <c r="D8" s="46">
+      <c r="D8" s="26">
         <v>25</v>
       </c>
-      <c r="E8" s="46">
-        <v>0</v>
-      </c>
-      <c r="F8" s="45">
-        <v>23</v>
-      </c>
-      <c r="G8" s="44" t="s">
+      <c r="E8" s="26">
+        <v>0</v>
+      </c>
+      <c r="F8" s="25">
+        <v>23</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
-      <c r="B9" s="44">
+      <c r="A9" s="14"/>
+      <c r="B9" s="24">
         <v>5</v>
       </c>
-      <c r="C9" s="45">
+      <c r="C9" s="25">
         <v>1960</v>
       </c>
-      <c r="D9" s="46">
-        <v>1</v>
-      </c>
-      <c r="E9" s="46">
-        <v>0</v>
-      </c>
-      <c r="F9" s="45">
-        <v>23</v>
-      </c>
-      <c r="G9" s="44" t="s">
+      <c r="D9" s="26">
+        <v>1</v>
+      </c>
+      <c r="E9" s="26">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25">
+        <v>23</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="44">
+      <c r="A10" s="14"/>
+      <c r="B10" s="24">
         <v>5</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="25">
         <v>1960</v>
       </c>
-      <c r="D10" s="46">
-        <v>1</v>
-      </c>
-      <c r="E10" s="46">
+      <c r="D10" s="26">
+        <v>1</v>
+      </c>
+      <c r="E10" s="26">
         <v>24</v>
       </c>
-      <c r="F10" s="45">
-        <v>23</v>
-      </c>
-      <c r="G10" s="44" t="s">
+      <c r="F10" s="25">
+        <v>23</v>
+      </c>
+      <c r="G10" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="44">
+      <c r="A11" s="14"/>
+      <c r="B11" s="24">
         <v>20</v>
       </c>
-      <c r="C11" s="45">
+      <c r="C11" s="25">
         <v>1960</v>
       </c>
-      <c r="D11" s="46">
+      <c r="D11" s="26">
         <v>100</v>
       </c>
-      <c r="E11" s="46">
-        <v>0</v>
-      </c>
-      <c r="F11" s="45">
-        <v>23</v>
-      </c>
-      <c r="G11" s="44" t="s">
+      <c r="E11" s="26">
+        <v>0</v>
+      </c>
+      <c r="F11" s="25">
+        <v>23</v>
+      </c>
+      <c r="G11" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="44">
+      <c r="A12" s="14"/>
+      <c r="B12" s="24">
         <v>20</v>
       </c>
-      <c r="C12" s="45">
+      <c r="C12" s="25">
         <v>1960</v>
       </c>
-      <c r="D12" s="46">
-        <v>1</v>
-      </c>
-      <c r="E12" s="46">
-        <v>0</v>
-      </c>
-      <c r="F12" s="45">
-        <v>23</v>
-      </c>
-      <c r="G12" s="44" t="s">
+      <c r="D12" s="26">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25">
+        <v>23</v>
+      </c>
+      <c r="G12" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
-      <c r="B13" s="44">
+      <c r="A13" s="14"/>
+      <c r="B13" s="24">
         <v>20</v>
       </c>
-      <c r="C13" s="45">
+      <c r="C13" s="25">
         <v>1960</v>
       </c>
-      <c r="D13" s="46">
-        <v>1</v>
-      </c>
-      <c r="E13" s="46">
+      <c r="D13" s="26">
+        <v>1</v>
+      </c>
+      <c r="E13" s="26">
         <v>99</v>
       </c>
-      <c r="F13" s="45">
-        <v>23</v>
-      </c>
-      <c r="G13" s="44" t="s">
+      <c r="F13" s="25">
+        <v>23</v>
+      </c>
+      <c r="G13" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
-      <c r="B14" s="47">
+      <c r="A14" s="14"/>
+      <c r="B14" s="27">
         <v>1.4</v>
       </c>
-      <c r="C14" s="48">
+      <c r="C14" s="28">
         <v>1989.3</v>
       </c>
-      <c r="D14" s="49">
-        <v>1</v>
-      </c>
-      <c r="E14" s="49">
-        <v>0</v>
-      </c>
-      <c r="F14" s="48">
-        <v>23</v>
-      </c>
-      <c r="G14" s="47" t="s">
+      <c r="D14" s="29">
+        <v>1</v>
+      </c>
+      <c r="E14" s="29">
+        <v>0</v>
+      </c>
+      <c r="F14" s="28">
+        <v>23</v>
+      </c>
+      <c r="G14" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="47">
+      <c r="A15" s="14"/>
+      <c r="B15" s="27">
         <v>1.4</v>
       </c>
-      <c r="C15" s="48">
+      <c r="C15" s="28">
         <v>1989.3</v>
       </c>
-      <c r="D15" s="49">
-        <v>1</v>
-      </c>
-      <c r="E15" s="49">
+      <c r="D15" s="29">
+        <v>1</v>
+      </c>
+      <c r="E15" s="29">
         <v>5</v>
       </c>
-      <c r="F15" s="48">
-        <v>23</v>
-      </c>
-      <c r="G15" s="47" t="s">
+      <c r="F15" s="28">
+        <v>23</v>
+      </c>
+      <c r="G15" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="47">
+      <c r="A16" s="14"/>
+      <c r="B16" s="27">
         <v>20</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="28">
         <v>1980</v>
       </c>
-      <c r="D16" s="49">
+      <c r="D16" s="29">
         <v>100</v>
       </c>
-      <c r="E16" s="49">
-        <v>0</v>
-      </c>
-      <c r="F16" s="48">
-        <v>23</v>
-      </c>
-      <c r="G16" s="47" t="s">
+      <c r="E16" s="29">
+        <v>0</v>
+      </c>
+      <c r="F16" s="28">
+        <v>23</v>
+      </c>
+      <c r="G16" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="47">
+      <c r="A17" s="14"/>
+      <c r="B17" s="27">
         <v>20</v>
       </c>
-      <c r="C17" s="48">
+      <c r="C17" s="28">
         <v>1980</v>
       </c>
-      <c r="D17" s="49">
-        <v>1</v>
-      </c>
-      <c r="E17" s="49">
-        <v>0</v>
-      </c>
-      <c r="F17" s="48">
-        <v>23</v>
-      </c>
-      <c r="G17" s="47" t="s">
+      <c r="D17" s="29">
+        <v>1</v>
+      </c>
+      <c r="E17" s="29">
+        <v>0</v>
+      </c>
+      <c r="F17" s="28">
+        <v>23</v>
+      </c>
+      <c r="G17" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
-      <c r="B18" s="47">
+      <c r="A18" s="14"/>
+      <c r="B18" s="27">
         <v>20</v>
       </c>
-      <c r="C18" s="48">
+      <c r="C18" s="28">
         <v>1980</v>
       </c>
-      <c r="D18" s="49">
-        <v>1</v>
-      </c>
-      <c r="E18" s="49">
+      <c r="D18" s="29">
+        <v>1</v>
+      </c>
+      <c r="E18" s="29">
         <v>99</v>
       </c>
-      <c r="F18" s="48">
-        <v>23</v>
-      </c>
-      <c r="G18" s="47" t="s">
+      <c r="F18" s="28">
+        <v>23</v>
+      </c>
+      <c r="G18" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="27">
+      <c r="A20" s="14">
         <v>4</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="41">
+      <c r="A21" s="14"/>
+      <c r="B21" s="21">
         <v>1.4</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="19">
         <v>2132.5</v>
       </c>
-      <c r="D21" s="43">
-        <v>1</v>
-      </c>
-      <c r="E21" s="43">
-        <v>0</v>
-      </c>
-      <c r="F21" s="42">
-        <v>23</v>
-      </c>
-      <c r="G21" s="44" t="s">
+      <c r="D21" s="23">
+        <v>1</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0</v>
+      </c>
+      <c r="F21" s="22">
+        <v>23</v>
+      </c>
+      <c r="G21" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27"/>
-      <c r="B22" s="44">
+      <c r="A22" s="14"/>
+      <c r="B22" s="24">
         <v>1.4</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="19">
         <v>2132.5</v>
       </c>
-      <c r="D22" s="46">
-        <v>1</v>
-      </c>
-      <c r="E22" s="46">
+      <c r="D22" s="26">
+        <v>1</v>
+      </c>
+      <c r="E22" s="26">
         <v>5</v>
       </c>
-      <c r="F22" s="45">
-        <v>23</v>
-      </c>
-      <c r="G22" s="44" t="s">
+      <c r="F22" s="25">
+        <v>23</v>
+      </c>
+      <c r="G22" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="47">
+      <c r="A23" s="14"/>
+      <c r="B23" s="27">
         <v>1.4</v>
       </c>
-      <c r="C23" s="48">
+      <c r="C23" s="28">
         <v>2154.3000000000002</v>
       </c>
-      <c r="D23" s="49">
+      <c r="D23" s="29">
         <v>6</v>
       </c>
-      <c r="E23" s="49">
-        <v>0</v>
-      </c>
-      <c r="F23" s="48">
-        <v>23</v>
-      </c>
-      <c r="G23" s="47" t="s">
+      <c r="E23" s="29">
+        <v>0</v>
+      </c>
+      <c r="F23" s="28">
+        <v>23</v>
+      </c>
+      <c r="G23" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="47">
+      <c r="A24" s="14"/>
+      <c r="B24" s="27">
         <v>1.4</v>
       </c>
-      <c r="C24" s="48">
+      <c r="C24" s="28">
         <v>2154.3000000000002</v>
       </c>
-      <c r="D24" s="49">
-        <v>1</v>
-      </c>
-      <c r="E24" s="49">
-        <v>0</v>
-      </c>
-      <c r="F24" s="48">
-        <v>23</v>
-      </c>
-      <c r="G24" s="47" t="s">
+      <c r="D24" s="29">
+        <v>1</v>
+      </c>
+      <c r="E24" s="29">
+        <v>0</v>
+      </c>
+      <c r="F24" s="28">
+        <v>23</v>
+      </c>
+      <c r="G24" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="47">
+      <c r="A25" s="14"/>
+      <c r="B25" s="27">
         <v>1.4</v>
       </c>
-      <c r="C25" s="48">
+      <c r="C25" s="28">
         <v>2154.3000000000002</v>
       </c>
-      <c r="D25" s="49">
-        <v>1</v>
-      </c>
-      <c r="E25" s="49">
+      <c r="D25" s="29">
+        <v>1</v>
+      </c>
+      <c r="E25" s="29">
         <v>5</v>
       </c>
-      <c r="F25" s="48">
-        <v>23</v>
-      </c>
-      <c r="G25" s="47" t="s">
+      <c r="F25" s="28">
+        <v>23</v>
+      </c>
+      <c r="G25" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="47">
+      <c r="A26" s="14"/>
+      <c r="B26" s="27">
         <v>5</v>
       </c>
-      <c r="C26" s="48">
+      <c r="C26" s="28">
         <v>2152.5</v>
       </c>
-      <c r="D26" s="49">
+      <c r="D26" s="29">
         <v>25</v>
       </c>
-      <c r="E26" s="49">
-        <v>0</v>
-      </c>
-      <c r="F26" s="48">
-        <v>23</v>
-      </c>
-      <c r="G26" s="47" t="s">
+      <c r="E26" s="29">
+        <v>0</v>
+      </c>
+      <c r="F26" s="28">
+        <v>23</v>
+      </c>
+      <c r="G26" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="47">
+      <c r="A27" s="14"/>
+      <c r="B27" s="27">
         <v>5</v>
       </c>
-      <c r="C27" s="48">
+      <c r="C27" s="28">
         <v>2152.5</v>
       </c>
-      <c r="D27" s="49">
-        <v>1</v>
-      </c>
-      <c r="E27" s="49">
-        <v>0</v>
-      </c>
-      <c r="F27" s="48">
-        <v>23</v>
-      </c>
-      <c r="G27" s="47" t="s">
+      <c r="D27" s="29">
+        <v>1</v>
+      </c>
+      <c r="E27" s="29">
+        <v>0</v>
+      </c>
+      <c r="F27" s="28">
+        <v>23</v>
+      </c>
+      <c r="G27" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="47">
+      <c r="A28" s="14"/>
+      <c r="B28" s="27">
         <v>5</v>
       </c>
-      <c r="C28" s="48">
+      <c r="C28" s="28">
         <v>2152.5</v>
       </c>
-      <c r="D28" s="49">
-        <v>1</v>
-      </c>
-      <c r="E28" s="49">
+      <c r="D28" s="29">
+        <v>1</v>
+      </c>
+      <c r="E28" s="29">
         <v>24</v>
       </c>
-      <c r="F28" s="48">
-        <v>23</v>
-      </c>
-      <c r="G28" s="47" t="s">
+      <c r="F28" s="28">
+        <v>23</v>
+      </c>
+      <c r="G28" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="27">
+      <c r="A30" s="14">
         <v>5</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="50">
+      <c r="A31" s="14"/>
+      <c r="B31" s="30">
         <v>1.4</v>
       </c>
-      <c r="C31" s="50">
+      <c r="C31" s="30">
         <v>881.5</v>
       </c>
-      <c r="D31" s="51">
-        <v>1</v>
-      </c>
-      <c r="E31" s="52">
-        <v>0</v>
-      </c>
-      <c r="F31" s="50">
-        <v>23</v>
-      </c>
-      <c r="G31" s="26" t="s">
+      <c r="D31" s="31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="32">
+        <v>0</v>
+      </c>
+      <c r="F31" s="30">
+        <v>23</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="50">
+      <c r="A32" s="14"/>
+      <c r="B32" s="30">
         <v>1.4</v>
       </c>
-      <c r="C32" s="50">
+      <c r="C32" s="30">
         <v>881.5</v>
       </c>
-      <c r="D32" s="51">
-        <v>1</v>
-      </c>
-      <c r="E32" s="52">
+      <c r="D32" s="31">
+        <v>1</v>
+      </c>
+      <c r="E32" s="32">
         <v>5</v>
       </c>
-      <c r="F32" s="50">
-        <v>23</v>
-      </c>
-      <c r="G32" s="26" t="s">
+      <c r="F32" s="30">
+        <v>23</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="50">
+      <c r="A33" s="14"/>
+      <c r="B33" s="30">
         <v>1.4</v>
       </c>
-      <c r="C33" s="50">
+      <c r="C33" s="30">
         <v>893.3</v>
       </c>
-      <c r="D33" s="51">
-        <v>1</v>
-      </c>
-      <c r="E33" s="52">
-        <v>0</v>
-      </c>
-      <c r="F33" s="50">
-        <v>23</v>
-      </c>
-      <c r="G33" s="26" t="s">
+      <c r="D33" s="31">
+        <v>1</v>
+      </c>
+      <c r="E33" s="32">
+        <v>0</v>
+      </c>
+      <c r="F33" s="30">
+        <v>23</v>
+      </c>
+      <c r="G33" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="27"/>
-      <c r="B34" s="50">
+      <c r="A34" s="14"/>
+      <c r="B34" s="30">
         <v>1.4</v>
       </c>
-      <c r="C34" s="50">
+      <c r="C34" s="30">
         <v>893.3</v>
       </c>
-      <c r="D34" s="51">
-        <v>1</v>
-      </c>
-      <c r="E34" s="52">
+      <c r="D34" s="31">
+        <v>1</v>
+      </c>
+      <c r="E34" s="32">
         <v>5</v>
       </c>
-      <c r="F34" s="50">
-        <v>23</v>
-      </c>
-      <c r="G34" s="26" t="s">
+      <c r="F34" s="30">
+        <v>23</v>
+      </c>
+      <c r="G34" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="27"/>
-      <c r="B35" s="50">
+      <c r="A35" s="14"/>
+      <c r="B35" s="30">
         <v>10</v>
       </c>
-      <c r="C35" s="50">
+      <c r="C35" s="30">
         <v>889</v>
       </c>
-      <c r="D35" s="51">
-        <v>1</v>
-      </c>
-      <c r="E35" s="52">
+      <c r="D35" s="31">
+        <v>1</v>
+      </c>
+      <c r="E35" s="32">
         <v>49</v>
       </c>
-      <c r="F35" s="50">
-        <v>23</v>
-      </c>
-      <c r="G35" s="26" t="s">
+      <c r="F35" s="30">
+        <v>23</v>
+      </c>
+      <c r="G35" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="27">
+      <c r="A37" s="14">
         <v>12</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="38">
+      <c r="A38" s="14"/>
+      <c r="B38" s="18">
         <v>1.4</v>
       </c>
-      <c r="C38" s="39">
+      <c r="C38" s="19">
         <v>737.5</v>
       </c>
-      <c r="D38" s="40">
+      <c r="D38" s="20">
         <v>6</v>
       </c>
-      <c r="E38" s="40">
-        <v>0</v>
-      </c>
-      <c r="F38" s="39">
-        <v>23</v>
-      </c>
-      <c r="G38" s="38" t="s">
+      <c r="E38" s="20">
+        <v>0</v>
+      </c>
+      <c r="F38" s="19">
+        <v>23</v>
+      </c>
+      <c r="G38" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="41">
+      <c r="A39" s="14"/>
+      <c r="B39" s="21">
         <v>1.4</v>
       </c>
-      <c r="C39" s="39">
+      <c r="C39" s="19">
         <v>737.5</v>
       </c>
-      <c r="D39" s="43">
-        <v>1</v>
-      </c>
-      <c r="E39" s="43">
-        <v>0</v>
-      </c>
-      <c r="F39" s="42">
-        <v>23</v>
-      </c>
-      <c r="G39" s="41" t="s">
+      <c r="D39" s="23">
+        <v>1</v>
+      </c>
+      <c r="E39" s="23">
+        <v>0</v>
+      </c>
+      <c r="F39" s="22">
+        <v>23</v>
+      </c>
+      <c r="G39" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
-      <c r="B40" s="41">
+      <c r="A40" s="14"/>
+      <c r="B40" s="21">
         <v>1.4</v>
       </c>
-      <c r="C40" s="39">
+      <c r="C40" s="19">
         <v>737.5</v>
       </c>
-      <c r="D40" s="43">
-        <v>1</v>
-      </c>
-      <c r="E40" s="43">
+      <c r="D40" s="23">
+        <v>1</v>
+      </c>
+      <c r="E40" s="23">
         <v>5</v>
       </c>
-      <c r="F40" s="42">
-        <v>23</v>
-      </c>
-      <c r="G40" s="41" t="s">
+      <c r="F40" s="22">
+        <v>23</v>
+      </c>
+      <c r="G40" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="27"/>
-      <c r="B41" s="47">
+      <c r="A41" s="14"/>
+      <c r="B41" s="27">
         <v>1.4</v>
       </c>
-      <c r="C41" s="48">
+      <c r="C41" s="28">
         <v>745.3</v>
       </c>
-      <c r="D41" s="49">
-        <v>1</v>
-      </c>
-      <c r="E41" s="49">
-        <v>0</v>
-      </c>
-      <c r="F41" s="48">
-        <v>23</v>
-      </c>
-      <c r="G41" s="47" t="s">
+      <c r="D41" s="29">
+        <v>1</v>
+      </c>
+      <c r="E41" s="29">
+        <v>0</v>
+      </c>
+      <c r="F41" s="28">
+        <v>23</v>
+      </c>
+      <c r="G41" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="27"/>
-      <c r="B42" s="47">
+      <c r="A42" s="14"/>
+      <c r="B42" s="27">
         <v>1.4</v>
       </c>
-      <c r="C42" s="48">
+      <c r="C42" s="28">
         <v>745.3</v>
       </c>
-      <c r="D42" s="49">
-        <v>1</v>
-      </c>
-      <c r="E42" s="49">
+      <c r="D42" s="29">
+        <v>1</v>
+      </c>
+      <c r="E42" s="29">
         <v>5</v>
       </c>
-      <c r="F42" s="48">
-        <v>23</v>
-      </c>
-      <c r="G42" s="47" t="s">
+      <c r="F42" s="28">
+        <v>23</v>
+      </c>
+      <c r="G42" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="A43" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
-      <c r="B44" s="41">
+      <c r="A44" s="14"/>
+      <c r="B44" s="21">
         <v>1.4</v>
       </c>
-      <c r="C44" s="39">
+      <c r="C44" s="19">
         <v>2145</v>
       </c>
-      <c r="D44" s="43">
-        <v>1</v>
-      </c>
-      <c r="E44" s="43">
-        <v>0</v>
-      </c>
-      <c r="F44" s="42">
-        <v>23</v>
-      </c>
-      <c r="G44" s="41" t="s">
+      <c r="D44" s="23">
+        <v>1</v>
+      </c>
+      <c r="E44" s="23">
+        <v>0</v>
+      </c>
+      <c r="F44" s="22">
+        <v>23</v>
+      </c>
+      <c r="G44" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="44">
+      <c r="A45" s="14"/>
+      <c r="B45" s="24">
         <v>1.4</v>
       </c>
-      <c r="C45" s="39">
+      <c r="C45" s="19">
         <v>2145</v>
       </c>
-      <c r="D45" s="46">
-        <v>1</v>
-      </c>
-      <c r="E45" s="46">
+      <c r="D45" s="26">
+        <v>1</v>
+      </c>
+      <c r="E45" s="26">
         <v>5</v>
       </c>
-      <c r="F45" s="45">
-        <v>23</v>
-      </c>
-      <c r="G45" s="44" t="s">
+      <c r="F45" s="25">
+        <v>23</v>
+      </c>
+      <c r="G45" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="27"/>
-      <c r="B46" s="47">
+      <c r="A46" s="14"/>
+      <c r="B46" s="27">
         <v>1.4</v>
       </c>
-      <c r="C46" s="48">
+      <c r="C46" s="28">
         <v>2179.3000000000002</v>
       </c>
-      <c r="D46" s="49">
-        <v>1</v>
-      </c>
-      <c r="E46" s="49">
-        <v>0</v>
-      </c>
-      <c r="F46" s="48">
-        <v>23</v>
-      </c>
-      <c r="G46" s="47" t="s">
+      <c r="D46" s="29">
+        <v>1</v>
+      </c>
+      <c r="E46" s="29">
+        <v>0</v>
+      </c>
+      <c r="F46" s="28">
+        <v>23</v>
+      </c>
+      <c r="G46" s="27" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
-      <c r="B47" s="47">
+      <c r="A47" s="14"/>
+      <c r="B47" s="27">
         <v>1.4</v>
       </c>
-      <c r="C47" s="48">
+      <c r="C47" s="28">
         <v>2179.3000000000002</v>
       </c>
-      <c r="D47" s="49">
-        <v>1</v>
-      </c>
-      <c r="E47" s="49">
+      <c r="D47" s="29">
+        <v>1</v>
+      </c>
+      <c r="E47" s="29">
         <v>5</v>
       </c>
-      <c r="F47" s="48">
-        <v>23</v>
-      </c>
-      <c r="G47" s="47" t="s">
+      <c r="F47" s="28">
+        <v>23</v>
+      </c>
+      <c r="G47" s="27" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modified:   Maxpowerinputfile.xlsx 	modified:   Minpowerinputfile.xlsx
</commit_message>
<xml_diff>
--- a/Maxpowerinputfile.xlsx
+++ b/Maxpowerinputfile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\LTE_RX_logging\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Test\DVT-Wireless-HCL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776D0133-6149-4105-8104-900F7D5C9253}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730F2EBE-62B1-4827-BE9C-071CFF3BB96A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2925" yWindow="945" windowWidth="25500" windowHeight="14265" xr2:uid="{BA741C37-369C-4D69-BC66-4EE94A3A8637}"/>
   </bookViews>

</xml_diff>